<commit_message>
Updated Character_Attribute_Data with Pyra and Mythra's data.
</commit_message>
<xml_diff>
--- a/Character_Attribute_Data.xlsx
+++ b/Character_Attribute_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\ICs SSBU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22355BD-FDE0-42AC-BA4D-243CB47FB5C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413A4FEC-FE6E-4167-9F30-5A4F17B297F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10365" yWindow="1470" windowWidth="12060" windowHeight="7665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="2265" windowWidth="12060" windowHeight="7665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Character</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Sephiroth (Winged Mode)</t>
+  </si>
+  <si>
+    <t>Mythra</t>
+  </si>
+  <si>
+    <t>Pyra</t>
   </si>
 </sst>
 </file>
@@ -677,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2201,18 +2207,18 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E59">
-        <v>7.6999999999999999E-2</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="F59">
-        <v>1.31</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2221,18 +2227,18 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E60">
-        <v>6.8000000000000005E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F60">
-        <v>1.35</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2241,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E61">
-        <v>7.1999999999999995E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F61">
         <v>1.35</v>
@@ -2252,7 +2258,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2261,18 +2267,18 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E62">
-        <v>0.12</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="F62">
-        <v>1.55</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2281,18 +2287,18 @@
         <v>1</v>
       </c>
       <c r="D63">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E63">
-        <v>7.0000000000000007E-2</v>
+        <v>0.12</v>
       </c>
       <c r="F63">
-        <v>1.19</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2301,18 +2307,18 @@
         <v>1</v>
       </c>
       <c r="D64">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="E64">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F64">
-        <v>1.9</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2321,18 +2327,18 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E65">
-        <v>9.5000000000000001E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F65">
-        <v>1.55</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2341,18 +2347,18 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="E66">
-        <v>0.14000000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="F66">
-        <v>1.95</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2361,18 +2367,18 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E67">
-        <v>8.1000000000000003E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F67">
-        <v>1.48</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2381,18 +2387,18 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E68">
-        <v>0.09</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F68">
-        <v>1.6</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2401,18 +2407,18 @@
         <v>1</v>
       </c>
       <c r="D69">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E69">
-        <v>8.5000000000000006E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F69">
-        <v>1.85</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2421,18 +2427,18 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E70">
         <v>0.09</v>
       </c>
       <c r="F70">
-        <v>1.78</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2441,18 +2447,18 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E71">
-        <v>8.8999999999999996E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F71">
-        <v>1.5</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2461,18 +2467,18 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E72">
-        <v>6.2E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F72">
-        <v>1.2</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2484,15 +2490,15 @@
         <v>95</v>
       </c>
       <c r="E73">
-        <v>0.114</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F73">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2501,18 +2507,18 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E74">
-        <v>0.12</v>
+        <v>6.2E-2</v>
       </c>
       <c r="F74">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2521,18 +2527,18 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E75">
-        <v>7.4999999999999997E-2</v>
+        <v>0.114</v>
       </c>
       <c r="F75">
-        <v>1.33</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2541,38 +2547,38 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E76">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="F76">
-        <v>1.84</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
         <v>108</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>79</v>
-      </c>
       <c r="E77">
-        <v>0.18540000000000001</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F77">
-        <v>1.9319999999999999</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2581,18 +2587,18 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E78">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="F78">
-        <v>1.75</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2601,38 +2607,38 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E79">
-        <v>9.8000000000000004E-2</v>
+        <v>0.18540000000000001</v>
       </c>
       <c r="F79">
-        <v>1.58</v>
+        <v>1.9319999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B80">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E80">
-        <v>0.13719999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F80">
-        <v>2.2120000000000002</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2644,7 +2650,7 @@
         <v>97</v>
       </c>
       <c r="E81">
-        <v>0.1176</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F81">
         <v>1.58</v>
@@ -2652,30 +2658,30 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B82">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="C82">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>97</v>
       </c>
       <c r="E82">
-        <v>9.8000000000000004E-2</v>
+        <v>0.13719999999999999</v>
       </c>
       <c r="F82">
-        <v>1.58</v>
+        <v>2.2120000000000002</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B83">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2684,7 +2690,7 @@
         <v>97</v>
       </c>
       <c r="E83">
-        <v>9.8000000000000004E-2</v>
+        <v>0.1176</v>
       </c>
       <c r="F83">
         <v>1.58</v>
@@ -2692,13 +2698,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C84">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="D84">
         <v>97</v>
@@ -2712,47 +2718,47 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E85">
-        <v>8.5000000000000006E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F85">
-        <v>1.85</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D86">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E86">
-        <v>0.08</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F86">
-        <v>1.73</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2761,18 +2767,18 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="E87">
-        <v>0.09</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F87">
-        <v>1.65</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2781,18 +2787,18 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="E88">
-        <v>0.128</v>
+        <v>0.08</v>
       </c>
       <c r="F88">
-        <v>1.35</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2801,18 +2807,18 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E89">
-        <v>7.0000000000000007E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F89">
-        <v>1.42</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2821,18 +2827,18 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="E90">
-        <v>0.09</v>
+        <v>0.128</v>
       </c>
       <c r="F90">
-        <v>1.48</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2841,18 +2847,18 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E91">
-        <v>8.1000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F91">
-        <v>1.38</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2861,18 +2867,18 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E92">
-        <v>7.8E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F92">
-        <v>1.32</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2881,18 +2887,18 @@
         <v>1</v>
       </c>
       <c r="D93">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E93">
-        <v>0.107</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F93">
-        <v>1.61</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2901,41 +2907,41 @@
         <v>1</v>
       </c>
       <c r="D94">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E94">
-        <v>0.09</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F94">
-        <v>1.3</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B95">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="E95">
-        <v>0.09</v>
+        <v>0.107</v>
       </c>
       <c r="F95">
-        <v>1.3</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B96">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2952,47 +2958,47 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E97">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="F97">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E98">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="F98">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -3001,10 +3007,10 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E99">
-        <v>9.6000000000000002E-2</v>
+        <v>0.13</v>
       </c>
       <c r="F99">
         <v>1.8</v>
@@ -3012,7 +3018,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -3021,32 +3027,72 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E100">
-        <v>7.0999999999999994E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F100">
-        <v>1.35</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>93</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>88</v>
+      </c>
+      <c r="E101">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F101">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>85</v>
+      </c>
+      <c r="E102">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F102">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>95</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101">
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
         <v>80</v>
       </c>
-      <c r="E101">
+      <c r="E103">
         <v>0.12</v>
       </c>
-      <c r="F101">
+      <c r="F103">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Kazuya attribute data.
</commit_message>
<xml_diff>
--- a/Character_Attribute_Data.xlsx
+++ b/Character_Attribute_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\ICs SSBU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\ICs SSBU\Calc Code\Github Clone\SSBU-ICs-Calc-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413A4FEC-FE6E-4167-9F30-5A4F17B297F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5F470E-D805-4962-B29B-5D1DECCA64D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="2265" windowWidth="12060" windowHeight="7665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Character</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Pyra</t>
+  </si>
+  <si>
+    <t>Kazuya</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1772,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1778,27 +1781,27 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E38">
-        <v>0.12</v>
+        <v>0.108</v>
       </c>
       <c r="F38">
-        <v>1.6</v>
+        <v>2.72</v>
       </c>
       <c r="G38">
-        <v>7.6600000000000001E-2</v>
+        <v>7.9967999999999997E-2</v>
       </c>
       <c r="H38">
         <v>1.8</v>
       </c>
       <c r="I38">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1807,18 +1810,27 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="E39">
-        <v>9.7000000000000003E-2</v>
+        <v>0.12</v>
       </c>
       <c r="F39">
-        <v>1.95</v>
+        <v>1.6</v>
+      </c>
+      <c r="G39">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="H39">
+        <v>1.8</v>
+      </c>
+      <c r="I39">
+        <v>0.11</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1838,7 +1850,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1847,18 +1859,18 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E41">
-        <v>0.105</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="F41">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1867,18 +1879,18 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="E42">
-        <v>6.4000000000000001E-2</v>
+        <v>0.105</v>
       </c>
       <c r="F42">
-        <v>1.23</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1887,18 +1899,18 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E43">
-        <v>9.6000000000000002E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F43">
-        <v>1.6</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1907,18 +1919,18 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E44">
-        <v>0.09</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F44">
-        <v>1.95</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1927,18 +1939,18 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E45">
-        <v>8.4000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F45">
-        <v>1.68</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1947,18 +1959,18 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E46">
-        <v>0.09</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="F46">
-        <v>1.37</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1967,18 +1979,18 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E47">
-        <v>7.4999999999999997E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F47">
-        <v>1.58</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1987,18 +1999,18 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E48">
-        <v>8.3000000000000004E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F48">
-        <v>1.32</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2007,18 +2019,18 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49">
-        <v>8.6999999999999994E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F49">
-        <v>1.5</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2027,18 +2039,18 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E50">
-        <v>7.4999999999999997E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="F50">
-        <v>1.58</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2047,18 +2059,18 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E51">
-        <v>0.107</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F51">
-        <v>1.8</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2067,18 +2079,18 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E52">
-        <v>0.11</v>
+        <v>0.107</v>
       </c>
       <c r="F52">
-        <v>1.66</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2087,78 +2099,78 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E53">
-        <v>8.2000000000000003E-2</v>
+        <v>0.11</v>
       </c>
       <c r="F53">
-        <v>1.55</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>79</v>
+      </c>
+      <c r="E54">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F54">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>50</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
         <v>94</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>0.16900000000000001</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>1.92</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
         <v>104</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F55">
+      <c r="F56">
         <v>1.45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>100</v>
-      </c>
-      <c r="E56">
-        <v>0.106</v>
-      </c>
-      <c r="F56">
-        <v>1.55</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2167,18 +2179,18 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E57">
-        <v>0.11</v>
+        <v>0.106</v>
       </c>
       <c r="F57">
-        <v>1.52</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2187,18 +2199,18 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="E58">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="F58">
-        <v>1.24</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2207,18 +2219,18 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E59">
-        <v>0.13700000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="F59">
-        <v>1.87</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2227,18 +2239,18 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E60">
-        <v>7.6999999999999999E-2</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="F60">
-        <v>1.31</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2247,18 +2259,18 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E61">
-        <v>6.8000000000000005E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F61">
-        <v>1.35</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2267,10 +2279,10 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E62">
-        <v>7.1999999999999995E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F62">
         <v>1.35</v>
@@ -2278,7 +2290,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2287,18 +2299,18 @@
         <v>1</v>
       </c>
       <c r="D63">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E63">
-        <v>0.12</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="F63">
-        <v>1.55</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2307,18 +2319,18 @@
         <v>1</v>
       </c>
       <c r="D64">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E64">
-        <v>7.0000000000000007E-2</v>
+        <v>0.12</v>
       </c>
       <c r="F64">
-        <v>1.19</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2327,18 +2339,18 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="E65">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F65">
-        <v>1.9</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2347,18 +2359,18 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E66">
-        <v>9.5000000000000001E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F66">
-        <v>1.55</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2367,18 +2379,18 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="E67">
-        <v>0.14000000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="F67">
-        <v>1.95</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2387,18 +2399,18 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E68">
-        <v>8.1000000000000003E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F68">
-        <v>1.48</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2407,18 +2419,18 @@
         <v>1</v>
       </c>
       <c r="D69">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E69">
-        <v>7.8E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F69">
-        <v>1.62</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2427,18 +2439,18 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E70">
-        <v>0.09</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F70">
-        <v>1.6</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2447,18 +2459,18 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E71">
-        <v>8.5000000000000006E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F71">
-        <v>1.85</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2470,15 +2482,15 @@
         <v>107</v>
       </c>
       <c r="E72">
-        <v>0.09</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F72">
-        <v>1.78</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2487,18 +2499,18 @@
         <v>1</v>
       </c>
       <c r="D73">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E73">
-        <v>8.8999999999999996E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F73">
-        <v>1.5</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2507,18 +2519,18 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E74">
-        <v>6.2E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F74">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2527,18 +2539,18 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E75">
-        <v>0.114</v>
+        <v>6.2E-2</v>
       </c>
       <c r="F75">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2547,18 +2559,18 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E76">
-        <v>0.12</v>
+        <v>0.114</v>
       </c>
       <c r="F76">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2567,18 +2579,18 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E77">
-        <v>7.4999999999999997E-2</v>
+        <v>0.12</v>
       </c>
       <c r="F77">
-        <v>1.33</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2587,18 +2599,18 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E78">
-        <v>0.18</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F78">
-        <v>1.84</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2610,15 +2622,15 @@
         <v>79</v>
       </c>
       <c r="E79">
-        <v>0.18540000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="F79">
-        <v>1.9319999999999999</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2627,18 +2639,18 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E80">
-        <v>0.15</v>
+        <v>0.18540000000000001</v>
       </c>
       <c r="F80">
-        <v>1.75</v>
+        <v>1.9319999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2647,21 +2659,21 @@
         <v>1</v>
       </c>
       <c r="D81">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E81">
-        <v>9.8000000000000004E-2</v>
+        <v>0.15</v>
       </c>
       <c r="F81">
-        <v>1.58</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2670,18 +2682,18 @@
         <v>97</v>
       </c>
       <c r="E82">
-        <v>0.13719999999999999</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F82">
-        <v>2.2120000000000002</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2690,27 +2702,27 @@
         <v>97</v>
       </c>
       <c r="E83">
-        <v>0.1176</v>
+        <v>0.13719999999999999</v>
       </c>
       <c r="F83">
-        <v>1.58</v>
+        <v>2.2120000000000002</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>97</v>
       </c>
       <c r="E84">
-        <v>9.8000000000000004E-2</v>
+        <v>0.1176</v>
       </c>
       <c r="F84">
         <v>1.58</v>
@@ -2718,13 +2730,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B85">
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D85">
         <v>97</v>
@@ -2738,13 +2750,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C86">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>97</v>
@@ -2758,27 +2770,27 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D87">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E87">
-        <v>8.5000000000000006E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F87">
-        <v>1.85</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2787,18 +2799,18 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E88">
-        <v>0.08</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F88">
-        <v>1.73</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2807,18 +2819,18 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="E89">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F89">
-        <v>1.65</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2827,18 +2839,18 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E90">
-        <v>0.128</v>
+        <v>0.09</v>
       </c>
       <c r="F90">
-        <v>1.35</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2847,18 +2859,18 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E91">
-        <v>7.0000000000000007E-2</v>
+        <v>0.128</v>
       </c>
       <c r="F91">
-        <v>1.42</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2867,18 +2879,18 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E92">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F92">
-        <v>1.48</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2887,18 +2899,18 @@
         <v>1</v>
       </c>
       <c r="D93">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E93">
-        <v>8.1000000000000003E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F93">
-        <v>1.38</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2907,18 +2919,18 @@
         <v>1</v>
       </c>
       <c r="D94">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E94">
-        <v>7.8E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F94">
-        <v>1.32</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2927,18 +2939,18 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E95">
-        <v>0.107</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F95">
-        <v>1.61</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2947,21 +2959,21 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="E96">
-        <v>0.09</v>
+        <v>0.107</v>
       </c>
       <c r="F96">
-        <v>1.3</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2978,7 +2990,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98">
         <v>0.9</v>
@@ -2998,47 +3010,47 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E99">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="F99">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
         <v>92</v>
       </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-      <c r="C100">
-        <v>1</v>
-      </c>
-      <c r="D100">
-        <v>104</v>
-      </c>
       <c r="E100">
-        <v>0.08</v>
+        <v>0.13</v>
       </c>
       <c r="F100">
-        <v>1.29</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -3047,18 +3059,18 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E101">
-        <v>9.6000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F101">
-        <v>1.8</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -3067,32 +3079,52 @@
         <v>1</v>
       </c>
       <c r="D102">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E102">
-        <v>7.0999999999999994E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F102">
-        <v>1.35</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>85</v>
+      </c>
+      <c r="E103">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F103">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>95</v>
       </c>
-      <c r="B103">
-        <v>1</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-      <c r="D103">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
         <v>80</v>
       </c>
-      <c r="E103">
+      <c r="E104">
         <v>0.12</v>
       </c>
-      <c r="F103">
+      <c r="F104">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>